<commit_message>
correct datatype in input file
</commit_message>
<xml_diff>
--- a/data/Fall2018/db1-7_all-timepoints-runs/db3/17-genes_32-edges_db3_Sigmoid_estimation_all-timepoints_no-dHAP4-data.xlsx
+++ b/data/Fall2018/db1-7_all-timepoints-runs/db3/17-genes_32-edges_db3_Sigmoid_estimation_all-timepoints_no-dHAP4-data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D15B046-5199-4E7C-9646-A06700DFF09E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="6855" tabRatio="868" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="6855" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="1" r:id="rId1"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="76">
   <si>
     <t>cols regulators/rows targets</t>
   </si>
@@ -164,259 +170,103 @@
     <t>estimate_params</t>
   </si>
   <si>
-    <t>-0.2792</t>
-  </si>
-  <si>
-    <t>-0.2436</t>
-  </si>
-  <si>
-    <t>0.1581</t>
-  </si>
-  <si>
     <t>1.0793</t>
-  </si>
-  <si>
-    <t>-1.8448</t>
-  </si>
-  <si>
-    <t>-0.383</t>
-  </si>
-  <si>
-    <t>0.2693</t>
   </si>
   <si>
     <t>-0.2042</t>
   </si>
   <si>
-    <t>-0.4827</t>
-  </si>
-  <si>
     <t>1.4649</t>
-  </si>
-  <si>
-    <t>-0.7654</t>
-  </si>
-  <si>
-    <t>-1.1456</t>
   </si>
   <si>
     <t>-0.9423</t>
   </si>
   <si>
-    <t>2.3352</t>
-  </si>
-  <si>
     <t>-0.3518</t>
-  </si>
-  <si>
-    <t>0.5869</t>
-  </si>
-  <si>
-    <t>0.0341</t>
   </si>
   <si>
     <t>1.4453</t>
   </si>
   <si>
-    <t>-0.5607</t>
-  </si>
-  <si>
-    <t>0.1712</t>
-  </si>
-  <si>
-    <t>-1.463</t>
-  </si>
-  <si>
-    <t>0.3025</t>
-  </si>
-  <si>
     <t>-0.0617</t>
-  </si>
-  <si>
-    <t>2.2291</t>
   </si>
   <si>
     <t>1.2958</t>
   </si>
   <si>
-    <t>1.5911</t>
-  </si>
-  <si>
-    <t>1.2566</t>
-  </si>
-  <si>
     <t>-3.5699</t>
-  </si>
-  <si>
-    <t>-0.345</t>
   </si>
   <si>
     <t>0.4422</t>
   </si>
   <si>
-    <t>1.8072</t>
-  </si>
-  <si>
-    <t>-0.8927</t>
-  </si>
-  <si>
     <t>1.1069</t>
-  </si>
-  <si>
-    <t>0.3945</t>
   </si>
   <si>
     <t>0.3325</t>
   </si>
   <si>
-    <t>0.6703</t>
-  </si>
-  <si>
-    <t>0.7164</t>
-  </si>
-  <si>
     <t>0.3263</t>
-  </si>
-  <si>
-    <t>1.9784</t>
   </si>
   <si>
     <t>-0.5489</t>
   </si>
   <si>
-    <t>-0.5302</t>
-  </si>
-  <si>
-    <t>0.016</t>
-  </si>
-  <si>
     <t>-0.04</t>
-  </si>
-  <si>
-    <t>0.3902</t>
   </si>
   <si>
     <t>1.5125</t>
   </si>
   <si>
-    <t>-0.0775</t>
-  </si>
-  <si>
-    <t>-0.522</t>
-  </si>
-  <si>
     <t>-1.1526</t>
-  </si>
-  <si>
-    <t>1.353</t>
   </si>
   <si>
     <t>0.4726</t>
   </si>
   <si>
-    <t>0.5256</t>
-  </si>
-  <si>
-    <t>-0.3325</t>
-  </si>
-  <si>
     <t>1.4622</t>
-  </si>
-  <si>
-    <t>-0.9051</t>
   </si>
   <si>
     <t>1.0717</t>
   </si>
   <si>
-    <t>-1.9025</t>
-  </si>
-  <si>
-    <t>-0.4406</t>
-  </si>
-  <si>
     <t>-2.2715</t>
-  </si>
-  <si>
-    <t>0.2188</t>
-  </si>
-  <si>
-    <t>2.5266</t>
-  </si>
-  <si>
-    <t>0.4041</t>
   </si>
   <si>
     <t>0.0511</t>
   </si>
   <si>
-    <t>-0.5177</t>
-  </si>
-  <si>
     <t>0.1802</t>
-  </si>
-  <si>
-    <t>0.8526</t>
-  </si>
-  <si>
-    <t>-0.4332</t>
   </si>
   <si>
     <t>1.146</t>
   </si>
   <si>
-    <t>-0.8535</t>
-  </si>
-  <si>
     <t>0.3344</t>
-  </si>
-  <si>
-    <t>-1.2684</t>
-  </si>
-  <si>
-    <t>-0.8782</t>
   </si>
   <si>
     <t>-0.802</t>
   </si>
   <si>
-    <t>1.2361</t>
-  </si>
-  <si>
     <t>-0.9354</t>
-  </si>
-  <si>
-    <t>-0.0589</t>
-  </si>
-  <si>
-    <t>-0.7158</t>
   </si>
   <si>
     <t>0.4284</t>
   </si>
   <si>
-    <t>-1.0332</t>
-  </si>
-  <si>
     <t>0.8398</t>
-  </si>
-  <si>
-    <t>2.3845</t>
-  </si>
-  <si>
-    <t>0.1525</t>
   </si>
   <si>
     <t>1.0756</t>
   </si>
   <si>
-    <t>0.9658</t>
+    <t>`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -462,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -471,10 +321,11 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,7 +383,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -565,9 +416,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,6 +468,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -775,19 +660,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.1328125" style="2"/>
+    <col min="2" max="2" width="15.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -795,7 +680,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -803,7 +688,7 @@
         <v>0.22359999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -811,7 +696,7 @@
         <v>0.20100000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -819,7 +704,7 @@
         <v>0.19259999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -827,7 +712,7 @@
         <v>0.32240000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -835,7 +720,7 @@
         <v>0.27179999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -843,7 +728,7 @@
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -851,7 +736,7 @@
         <v>0.17119999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -859,7 +744,7 @@
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -867,7 +752,7 @@
         <v>0.4078</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -875,7 +760,7 @@
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -883,7 +768,7 @@
         <v>0.69320000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -891,7 +776,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -899,7 +784,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -907,7 +792,7 @@
         <v>0.32240000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -915,7 +800,7 @@
         <v>0.17319999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -923,7 +808,7 @@
         <v>0.72960000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -938,20 +823,20 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B3" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="14" width="9.265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -959,7 +844,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -967,7 +852,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -975,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -983,7 +868,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -991,7 +876,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -999,7 +884,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1007,7 +892,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1015,7 +900,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>43</v>
       </c>
@@ -1023,7 +908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1031,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1039,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -1047,7 +932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1055,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -1075,7 +960,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1095,7 +980,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1181,19 +1066,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.1328125" style="2"/>
+    <col min="2" max="2" width="10.59765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1201,7 +1086,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1209,7 +1094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1217,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1225,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1233,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1241,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1249,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1257,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1265,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1273,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1281,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1289,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1305,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1313,7 +1198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1321,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1329,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1343,17 +1228,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1361,7 +1246,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1369,7 +1254,7 @@
         <v>0.1118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1377,7 +1262,7 @@
         <v>0.10050000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1385,7 +1270,7 @@
         <v>9.6299999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1393,7 +1278,7 @@
         <v>0.16120000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1401,7 +1286,7 @@
         <v>0.13589999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1409,7 +1294,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1417,7 +1302,7 @@
         <v>8.5599999999999996E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1425,7 +1310,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1318,7 @@
         <v>0.2039</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1441,7 +1326,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1449,7 +1334,7 @@
         <v>0.34660000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1457,7 +1342,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1465,7 +1350,7 @@
         <v>0.14149999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1473,7 +1358,7 @@
         <v>0.16120000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1481,7 +1366,7 @@
         <v>8.6599999999999996E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1489,7 +1374,7 @@
         <v>0.36480000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1503,19 +1388,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="24" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="24" width="7.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -1589,7 +1476,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1659,7 +1546,7 @@
         <v>-0.31900000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1733,7 +1620,7 @@
         <v>1.0625</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1807,7 +1694,7 @@
         <v>-1.1623000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1881,7 +1768,7 @@
         <v>-1.4531000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1955,7 +1842,7 @@
         <v>-1.0219</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2029,7 +1916,7 @@
         <v>0.7853</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2103,7 +1990,7 @@
         <v>0.20930000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2177,7 +2064,7 @@
         <v>1.2694000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2251,7 +2138,7 @@
         <v>0.47389999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2325,7 +2212,7 @@
         <v>0.59889999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2399,7 +2286,7 @@
         <v>0.40789999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2473,7 +2360,7 @@
         <v>-0.47739999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2547,7 +2434,7 @@
         <v>-0.95709999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -2621,7 +2508,7 @@
         <v>0.51490000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2693,7 +2580,7 @@
       </c>
       <c r="X16" s="7"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -2767,7 +2654,7 @@
         <v>-1.379</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -2846,21 +2733,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T18" activeCellId="8" sqref="C3 B10 C14 I2 J3 P9 S3 T8 T18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="7.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -2925,15 +2812,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>-0.17180000000000001</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>45</v>
+      <c r="C2" s="5">
+        <v>-0.2792</v>
       </c>
       <c r="D2" s="5">
         <v>-0.17519999999999999</v>
@@ -2941,11 +2828,11 @@
       <c r="E2" s="5">
         <v>-0.68840000000000001</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>47</v>
+      <c r="F2" s="8">
+        <v>-0.24360000000000001</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.15809999999999999</v>
       </c>
       <c r="H2" s="5">
         <v>-0.42530000000000001</v>
@@ -2976,7 +2863,7 @@
         <v>2.9009999999999998</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="S2" s="5">
         <v>0.89990000000000003</v>
@@ -2988,7 +2875,7 @@
         <v>-0.29010000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3002,11 +2889,11 @@
       <c r="E3" s="5">
         <v>-0.1191</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>51</v>
+      <c r="F3" s="8">
+        <v>-0.38300000000000001</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.26929999999999998</v>
       </c>
       <c r="H3" s="5">
         <v>-7.5700000000000003E-2</v>
@@ -3037,7 +2924,7 @@
         <v>0.55030000000000001</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="5">
@@ -3047,7 +2934,7 @@
         <v>0.185</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3055,7 +2942,7 @@
         <v>-0.3155</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D4" s="5">
         <v>-0.80289999999999995</v>
@@ -3063,11 +2950,11 @@
       <c r="E4" s="5">
         <v>0.5141</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>56</v>
+      <c r="F4" s="8">
+        <v>-0.76539999999999997</v>
+      </c>
+      <c r="G4" s="8">
+        <v>-1.1456</v>
       </c>
       <c r="H4" s="5">
         <v>0.50960000000000005</v>
@@ -3100,7 +2987,7 @@
         <v>-0.5786</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="S4" s="5">
         <v>0.78710000000000002</v>
@@ -3112,7 +2999,7 @@
         <v>0.14269999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3120,7 +3007,7 @@
         <v>0.96209999999999996</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D5" s="5">
         <v>0.31009999999999999</v>
@@ -3128,11 +3015,11 @@
       <c r="E5" s="5">
         <v>-0.15890000000000001</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>61</v>
+      <c r="F5" s="8">
+        <v>0.58689999999999998</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3.4099999999999998E-2</v>
       </c>
       <c r="H5" s="5">
         <v>0.48599999999999999</v>
@@ -3165,7 +3052,7 @@
         <v>-2.6499999999999999E-2</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="S5" s="5">
         <v>-1.0232000000000001</v>
@@ -3177,15 +3064,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>64</v>
+      <c r="C6" s="5">
+        <v>0.17119999999999999</v>
       </c>
       <c r="D6" s="5">
         <v>-1.9531000000000001</v>
@@ -3193,11 +3080,11 @@
       <c r="E6" s="5">
         <v>-0.21510000000000001</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>66</v>
+      <c r="F6" s="8">
+        <v>-1.4630000000000001</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.30249999999999999</v>
       </c>
       <c r="H6" s="5">
         <v>-2.2646000000000002</v>
@@ -3230,7 +3117,7 @@
         <v>-1.2024999999999999</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="S6" s="5">
         <v>1.1213</v>
@@ -3242,7 +3129,7 @@
         <v>1.583</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -3250,7 +3137,7 @@
         <v>-0.91690000000000005</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="D7" s="5">
         <v>0.42699999999999999</v>
@@ -3258,11 +3145,11 @@
       <c r="E7" s="5">
         <v>-7.1199999999999999E-2</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>71</v>
+      <c r="F7" s="8">
+        <v>1.5911</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1.2565999999999999</v>
       </c>
       <c r="H7" s="5">
         <v>0.39100000000000001</v>
@@ -3295,7 +3182,7 @@
         <v>1.099</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="S7" s="5">
         <v>-1.8355999999999999</v>
@@ -3307,7 +3194,7 @@
         <v>-2.9781</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3315,7 +3202,7 @@
         <v>0.48080000000000001</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D8" s="5">
         <v>1.4923999999999999</v>
@@ -3323,11 +3210,11 @@
       <c r="E8" s="5">
         <v>2.4096000000000002</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>76</v>
+      <c r="F8" s="8">
+        <v>1.8071999999999999</v>
+      </c>
+      <c r="G8" s="8">
+        <v>-0.89270000000000005</v>
       </c>
       <c r="H8" s="5">
         <v>0.75890000000000002</v>
@@ -3360,7 +3247,7 @@
         <v>0.5645</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="S8" s="5">
         <v>0.4713</v>
@@ -3370,7 +3257,7 @@
         <v>1.2195</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3378,7 +3265,7 @@
         <v>9.8199999999999996E-2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="D9" s="5">
         <v>0.29420000000000002</v>
@@ -3386,11 +3273,11 @@
       <c r="E9" s="5">
         <v>5.2299999999999999E-2</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>81</v>
+      <c r="F9" s="8">
+        <v>0.67030000000000001</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.71640000000000004</v>
       </c>
       <c r="H9" s="5">
         <v>0.33739999999999998</v>
@@ -3421,7 +3308,7 @@
         <v>-0.36409999999999998</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="S9" s="5">
         <v>-0.1216</v>
@@ -3433,13 +3320,13 @@
         <v>-0.113</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D10" s="5">
         <v>0.24909999999999999</v>
@@ -3447,11 +3334,11 @@
       <c r="E10" s="5">
         <v>0.90359999999999996</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>86</v>
+      <c r="F10" s="8">
+        <v>-0.5302</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1.6E-2</v>
       </c>
       <c r="H10" s="5">
         <v>-9.9699999999999997E-2</v>
@@ -3484,7 +3371,7 @@
         <v>0.41470000000000001</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="S10" s="5">
         <v>-0.1053</v>
@@ -3496,7 +3383,7 @@
         <v>1.0256000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3504,7 +3391,7 @@
         <v>0.58789999999999998</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="D11" s="5">
         <v>0.36570000000000003</v>
@@ -3512,11 +3399,11 @@
       <c r="E11" s="5">
         <v>0.68759999999999999</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>91</v>
+      <c r="F11" s="8">
+        <v>-7.7499999999999999E-2</v>
+      </c>
+      <c r="G11" s="8">
+        <v>-0.52200000000000002</v>
       </c>
       <c r="H11" s="5">
         <v>0.30730000000000002</v>
@@ -3549,7 +3436,7 @@
         <v>-0.28460000000000002</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="S11" s="5">
         <v>1.3992</v>
@@ -3561,7 +3448,7 @@
         <v>-0.68059999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -3569,7 +3456,7 @@
         <v>1.0931999999999999</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="D12" s="5">
         <v>1.1254999999999999</v>
@@ -3577,11 +3464,11 @@
       <c r="E12" s="5">
         <v>0.62629999999999997</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>96</v>
+      <c r="F12" s="8">
+        <v>0.52559999999999996</v>
+      </c>
+      <c r="G12" s="8">
+        <v>-0.33250000000000002</v>
       </c>
       <c r="H12" s="5">
         <v>1.6525000000000001</v>
@@ -3614,7 +3501,7 @@
         <v>-0.1474</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="S12" s="5">
         <v>3.78E-2</v>
@@ -3626,7 +3513,7 @@
         <v>0.20419999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -3634,7 +3521,7 @@
         <v>1.2589999999999999</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="D13" s="5">
         <v>0.91600000000000004</v>
@@ -3642,11 +3529,11 @@
       <c r="E13" s="5">
         <v>0.80400000000000005</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>101</v>
+      <c r="F13" s="8">
+        <v>-1.9025000000000001</v>
+      </c>
+      <c r="G13" s="8">
+        <v>-0.44059999999999999</v>
       </c>
       <c r="H13" s="5">
         <v>0.56589999999999996</v>
@@ -3679,7 +3566,7 @@
         <v>1.3001</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="S13" s="5">
         <v>-0.24709999999999999</v>
@@ -3691,7 +3578,7 @@
         <v>0.88700000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -3705,11 +3592,11 @@
       <c r="E14" s="5">
         <v>-0.54890000000000005</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>105</v>
+      <c r="F14" s="8">
+        <v>2.5266000000000002</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.40410000000000001</v>
       </c>
       <c r="H14" s="5">
         <v>2.5700000000000001E-2</v>
@@ -3742,7 +3629,7 @@
         <v>-7.9000000000000008E-3</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="S14" s="5">
         <v>0.57050000000000001</v>
@@ -3754,7 +3641,7 @@
         <v>-0.24779999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -3762,7 +3649,7 @@
         <v>-0.1331</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="D15" s="5">
         <v>-0.32140000000000002</v>
@@ -3770,11 +3657,11 @@
       <c r="E15" s="5">
         <v>-1.8200000000000001E-2</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>110</v>
+      <c r="F15" s="8">
+        <v>0.85260000000000002</v>
+      </c>
+      <c r="G15" s="8">
+        <v>-0.43319999999999997</v>
       </c>
       <c r="H15" s="5">
         <v>0.22489999999999999</v>
@@ -3807,7 +3694,7 @@
         <v>1.0215000000000001</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="S15" s="5">
         <v>-0.61909999999999998</v>
@@ -3819,7 +3706,7 @@
         <v>1.4060999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -3827,7 +3714,7 @@
         <v>-1.2421</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="D16" s="5">
         <v>-0.73499999999999999</v>
@@ -3835,11 +3722,11 @@
       <c r="E16" s="5">
         <v>0.29349999999999998</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>115</v>
+      <c r="F16" s="8">
+        <v>-1.2684</v>
+      </c>
+      <c r="G16" s="8">
+        <v>-0.87819999999999998</v>
       </c>
       <c r="H16" s="5">
         <v>1.0021</v>
@@ -3872,7 +3759,7 @@
         <v>-2.1100000000000001E-2</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="S16" s="5">
         <v>0.77529999999999999</v>
@@ -3884,7 +3771,7 @@
         <v>-0.2631</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -3892,7 +3779,7 @@
         <v>-1.3433999999999999</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="D17" s="5">
         <v>-1.7083999999999999</v>
@@ -3900,11 +3787,11 @@
       <c r="E17" s="5">
         <v>-0.28220000000000001</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>120</v>
+      <c r="F17" s="8">
+        <v>-5.8900000000000001E-2</v>
+      </c>
+      <c r="G17" s="8">
+        <v>-0.71579999999999999</v>
       </c>
       <c r="H17" s="5">
         <v>-0.11550000000000001</v>
@@ -3937,7 +3824,7 @@
         <v>1.3318000000000001</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="S17" s="5">
         <v>-0.67410000000000003</v>
@@ -3949,7 +3836,7 @@
         <v>-0.94159999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -3957,7 +3844,7 @@
         <v>0.83440000000000003</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="D18" s="5">
         <v>0.91839999999999999</v>
@@ -3965,11 +3852,11 @@
       <c r="E18" s="5">
         <v>0.47470000000000001</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>125</v>
+      <c r="F18" s="8">
+        <v>2.3845000000000001</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.1525</v>
       </c>
       <c r="H18" s="5">
         <v>0.65110000000000001</v>
@@ -4002,7 +3889,7 @@
         <v>0.61909999999999998</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="S18" s="5">
         <v>0.1502</v>
@@ -4010,6 +3897,11 @@
       <c r="T18" s="7"/>
       <c r="U18" s="5">
         <v>-4.1300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="F19" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -4018,19 +3910,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="7.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -4095,7 +3989,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4147,8 +4041,8 @@
       <c r="Q2" s="5">
         <v>2.0644</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>49</v>
+      <c r="R2" s="8">
+        <v>-1.8448</v>
       </c>
       <c r="S2" s="5">
         <v>4.2244000000000002</v>
@@ -4160,7 +4054,7 @@
         <v>0.35189999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4212,8 +4106,8 @@
       <c r="Q3" s="5">
         <v>2.3325</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>53</v>
+      <c r="R3" s="8">
+        <v>-0.48270000000000002</v>
       </c>
       <c r="S3" s="5">
         <v>1.7847999999999999</v>
@@ -4225,7 +4119,7 @@
         <v>5.1330999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4275,8 +4169,8 @@
       <c r="Q4" s="5">
         <v>-0.92279999999999995</v>
       </c>
-      <c r="R4" s="5" t="s">
-        <v>58</v>
+      <c r="R4" s="8">
+        <v>2.3351999999999999</v>
       </c>
       <c r="S4" s="5">
         <v>-0.33929999999999999</v>
@@ -4288,7 +4182,7 @@
         <v>-0.61240000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4340,8 +4234,8 @@
       <c r="Q5" s="5">
         <v>0.48330000000000001</v>
       </c>
-      <c r="R5" s="5" t="s">
-        <v>63</v>
+      <c r="R5" s="8">
+        <v>-0.56069999999999998</v>
       </c>
       <c r="S5" s="5">
         <v>3.3700000000000001E-2</v>
@@ -4353,7 +4247,7 @@
         <v>-0.97250000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -4405,8 +4299,8 @@
       <c r="Q6" s="5">
         <v>-0.86240000000000006</v>
       </c>
-      <c r="R6" s="5" t="s">
-        <v>68</v>
+      <c r="R6" s="8">
+        <v>2.2290999999999999</v>
       </c>
       <c r="S6" s="5">
         <v>1.0261</v>
@@ -4418,7 +4312,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -4470,8 +4364,8 @@
       <c r="Q7" s="5">
         <v>2.133</v>
       </c>
-      <c r="R7" s="5" t="s">
-        <v>73</v>
+      <c r="R7" s="8">
+        <v>-0.34499999999999997</v>
       </c>
       <c r="S7" s="5">
         <v>-2.0594999999999999</v>
@@ -4483,7 +4377,7 @@
         <v>-2.0489000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -4521,14 +4415,14 @@
         <v>-0.82179999999999997</v>
       </c>
       <c r="Q8" s="7"/>
-      <c r="R8" s="5" t="s">
-        <v>78</v>
+      <c r="R8" s="8">
+        <v>0.39450000000000002</v>
       </c>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -4580,8 +4474,8 @@
       <c r="Q9" s="5">
         <v>-2.5100000000000001E-2</v>
       </c>
-      <c r="R9" s="5" t="s">
-        <v>83</v>
+      <c r="R9" s="8">
+        <v>1.9783999999999999</v>
       </c>
       <c r="S9" s="5">
         <v>0.24010000000000001</v>
@@ -4593,7 +4487,7 @@
         <v>-0.77039999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -4643,8 +4537,8 @@
       <c r="Q10" s="5">
         <v>2.1431</v>
       </c>
-      <c r="R10" s="5" t="s">
-        <v>88</v>
+      <c r="R10" s="8">
+        <v>0.39019999999999999</v>
       </c>
       <c r="S10" s="5">
         <v>-0.41870000000000002</v>
@@ -4656,7 +4550,7 @@
         <v>0.55079999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -4708,8 +4602,8 @@
       <c r="Q11" s="5">
         <v>-0.3024</v>
       </c>
-      <c r="R11" s="5" t="s">
-        <v>93</v>
+      <c r="R11" s="8">
+        <v>1.353</v>
       </c>
       <c r="S11" s="5">
         <v>0.442</v>
@@ -4721,7 +4615,7 @@
         <v>-1.9781</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -4773,8 +4667,8 @@
       <c r="Q12" s="5">
         <v>1.2373000000000001</v>
       </c>
-      <c r="R12" s="5" t="s">
-        <v>98</v>
+      <c r="R12" s="8">
+        <v>-0.90510000000000002</v>
       </c>
       <c r="S12" s="5">
         <v>-0.53249999999999997</v>
@@ -4786,7 +4680,7 @@
         <v>-0.1676</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -4836,8 +4730,8 @@
       <c r="Q13" s="5">
         <v>-0.86599999999999999</v>
       </c>
-      <c r="R13" s="5" t="s">
-        <v>103</v>
+      <c r="R13" s="8">
+        <v>0.21879999999999999</v>
       </c>
       <c r="S13" s="5">
         <v>-0.92359999999999998</v>
@@ -4849,7 +4743,7 @@
         <v>-2.0510999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -4901,8 +4795,8 @@
       <c r="Q14" s="5">
         <v>0.21049999999999999</v>
       </c>
-      <c r="R14" s="5" t="s">
-        <v>107</v>
+      <c r="R14" s="8">
+        <v>-0.51770000000000005</v>
       </c>
       <c r="S14" s="5">
         <v>-0.45090000000000002</v>
@@ -4914,7 +4808,7 @@
         <v>-0.222</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -4964,8 +4858,8 @@
       <c r="Q15" s="5">
         <v>0.62970000000000004</v>
       </c>
-      <c r="R15" s="5" t="s">
-        <v>112</v>
+      <c r="R15" s="8">
+        <v>-0.85350000000000004</v>
       </c>
       <c r="S15" s="5">
         <v>0.29920000000000002</v>
@@ -4977,7 +4871,7 @@
         <v>-0.26190000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -5029,8 +4923,8 @@
       <c r="Q16" s="5">
         <v>0.2349</v>
       </c>
-      <c r="R16" s="5" t="s">
-        <v>117</v>
+      <c r="R16" s="8">
+        <v>1.2361</v>
       </c>
       <c r="S16" s="5">
         <v>-0.28249999999999997</v>
@@ -5042,7 +4936,7 @@
         <v>1.8572</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -5092,8 +4986,8 @@
       <c r="Q17" s="5">
         <v>3.3220000000000001</v>
       </c>
-      <c r="R17" s="5" t="s">
-        <v>122</v>
+      <c r="R17" s="8">
+        <v>-1.0331999999999999</v>
       </c>
       <c r="S17" s="5">
         <v>1.9711000000000001</v>
@@ -5105,7 +4999,7 @@
         <v>1.4166000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -5149,8 +5043,8 @@
       <c r="Q18" s="5">
         <v>0.50780000000000003</v>
       </c>
-      <c r="R18" s="5" t="s">
-        <v>127</v>
+      <c r="R18" s="8">
+        <v>0.96579999999999999</v>
       </c>
       <c r="S18" s="5">
         <v>6.6299999999999998E-2</v>
@@ -5168,19 +5062,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="7.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -5245,7 +5139,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -5310,7 +5204,7 @@
         <v>0.57740000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -5375,7 +5269,7 @@
         <v>-0.92689999999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -5440,7 +5334,7 @@
         <v>-1.0406</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -5505,7 +5399,7 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -5570,7 +5464,7 @@
         <v>0.47910000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -5635,7 +5529,7 @@
         <v>-2.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -5700,7 +5594,7 @@
         <v>-2.0543999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -5765,7 +5659,7 @@
         <v>0.1542</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -5830,7 +5724,7 @@
         <v>1.0784</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -5895,7 +5789,7 @@
         <v>1.7882</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -5960,7 +5854,7 @@
         <v>-0.50970000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -6005,7 +5899,7 @@
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -6070,7 +5964,7 @@
         <v>0.1336</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -6135,7 +6029,7 @@
         <v>0.11559999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -6200,7 +6094,7 @@
         <v>-2.7099999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -6265,7 +6159,7 @@
         <v>-0.86080000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -6336,19 +6230,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="7.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -6413,7 +6307,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -6478,7 +6372,7 @@
         <v>0.1575</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -6541,7 +6435,7 @@
         <v>1.4026000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -6606,7 +6500,7 @@
         <v>-0.3397</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -6671,7 +6565,7 @@
         <v>-0.55430000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -6736,7 +6630,7 @@
         <v>-8.2600000000000007E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -6801,7 +6695,7 @@
         <v>-1.9366000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -6860,7 +6754,7 @@
       </c>
       <c r="U8" s="7"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -6925,7 +6819,7 @@
         <v>0.14729999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -6990,7 +6884,7 @@
         <v>1.5842000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -7055,7 +6949,7 @@
         <v>-1.0366</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -7120,7 +7014,7 @@
         <v>-0.26100000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -7185,7 +7079,7 @@
         <v>-2.8431999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -7250,7 +7144,7 @@
         <v>-6.7799999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -7315,7 +7209,7 @@
         <v>1.43E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -7380,7 +7274,7 @@
         <v>0.47120000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -7445,7 +7339,7 @@
         <v>2.0861000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -7510,17 +7404,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7576,7 +7470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7632,7 +7526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -7688,7 +7582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -7744,7 +7638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -7800,7 +7694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -7856,7 +7750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -7912,7 +7806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -7968,7 +7862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -8024,7 +7918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -8080,7 +7974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -8136,7 +8030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -8192,7 +8086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -8248,7 +8142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -8304,7 +8198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -8360,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -8416,7 +8310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -8472,7 +8366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -8534,17 +8428,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8600,7 +8494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8656,7 +8550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -8712,7 +8606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -8768,7 +8662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -8824,7 +8718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -8880,7 +8774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -8936,7 +8830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -8992,7 +8886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -9048,7 +8942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -9104,7 +8998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -9160,7 +9054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -9216,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -9272,7 +9166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -9328,7 +9222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -9384,7 +9278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -9440,7 +9334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -9496,7 +9390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>

</xml_diff>